<commit_message>
C4 Q5 test sequence modified to reflect stuck at 1 errors
</commit_message>
<xml_diff>
--- a/C4/Data.xlsx
+++ b/C4/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Q3" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="68">
   <si>
     <t>A</t>
   </si>
@@ -579,25 +579,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -716,6 +697,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1180,25 +1180,25 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="32" t="s">
+      <c r="B12" s="74"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="33"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="11" t="s">
         <v>19</v>
       </c>
@@ -1496,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,31 +2011,31 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="32" t="s">
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="33"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="73"/>
       <c r="I20" s="21" t="s">
         <v>19</v>
       </c>
@@ -2572,28 +2572,152 @@
       <c r="B38" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="8">
-        <v>0</v>
-      </c>
-      <c r="D38" s="6">
+      <c r="C38" s="5">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9">
         <v>0</v>
       </c>
       <c r="E38" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="15">
         <v>0</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G38:G42" si="6">INT(OR(AND(NOT(E38),F38),AND(NOT(F38),D38)))</f>
         <v>0</v>
       </c>
       <c r="H38" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H38:H42" si="7">INT(AND(NOT(D38),F38))</f>
         <v>0</v>
       </c>
       <c r="I38" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>0</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="9">
+        <v>1</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1</v>
+      </c>
+      <c r="F39" s="15">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H39" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>0</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="8">
+        <v>0</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0</v>
+      </c>
+      <c r="E40" s="12">
+        <v>0</v>
+      </c>
+      <c r="F40" s="15">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="22" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>0</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+      <c r="D42" s="6">
+        <v>0</v>
+      </c>
+      <c r="E42" s="12">
+        <v>0</v>
+      </c>
+      <c r="F42" s="15">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H42" s="15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="22" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2644,14 +2768,14 @@
       <c r="J1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -2683,13 +2807,13 @@
       <c r="J2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -2861,29 +2985,29 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="32" t="s">
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
       <c r="H12" s="21" t="s">
         <v>19</v>
       </c>
@@ -3857,35 +3981,35 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="32" t="s">
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="33"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="73"/>
       <c r="K20" s="21" t="s">
         <v>19</v>
       </c>
@@ -4604,42 +4728,42 @@
     <col min="21" max="23" width="9.140625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="45" t="s">
+      <c r="I1" s="39"/>
+      <c r="J1" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="45" t="s">
+      <c r="K1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="40" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4657,19 +4781,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="16">
-        <f>INT(OR(AND(NOT(C2),D2),AND(C2,NOT(D2),A2)))</f>
+        <f t="shared" ref="E2:E17" si="0">INT(OR(AND(NOT(C2),D2),AND(C2,NOT(D2),A2)))</f>
         <v>0</v>
       </c>
       <c r="F2" s="17">
-        <f>INT(OR(AND(A2,NOT(D2),NOT(C2)),AND(NOT(A2),D2,NOT(C2))))</f>
+        <f t="shared" ref="F2:F17" si="1">INT(OR(AND(A2,NOT(D2),NOT(C2)),AND(NOT(A2),D2,NOT(C2))))</f>
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <f>INT(OR(AND(NOT(C2),D2),AND(NOT(D2),B2)))</f>
+        <f t="shared" ref="G2:G17" si="2">INT(OR(AND(NOT(C2),D2),AND(NOT(D2),B2)))</f>
         <v>0</v>
       </c>
       <c r="H2" s="2">
-        <f>INT(AND(NOT(B2),D2))</f>
+        <f t="shared" ref="H2:H17" si="3">INT(AND(NOT(B2),D2))</f>
         <v>0</v>
       </c>
       <c r="I2" s="25"/>
@@ -4700,19 +4824,19 @@
         <v>0</v>
       </c>
       <c r="E3" s="12">
-        <f>INT(OR(AND(NOT(C3),D3),AND(C3,NOT(D3),A3)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F3" s="15">
-        <f>INT(OR(AND(A3,NOT(D3),NOT(C3)),AND(NOT(A3),D3,NOT(C3))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G3" s="2">
-        <f>INT(OR(AND(NOT(C3),D3),AND(NOT(D3),B3)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H3" s="2">
-        <f>INT(AND(NOT(B3),D3))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I3" s="25"/>
@@ -4743,19 +4867,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="12">
-        <f>INT(OR(AND(NOT(C4),D4),AND(C4,NOT(D4),A4)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4" s="15">
-        <f>INT(OR(AND(A4,NOT(D4),NOT(C4)),AND(NOT(A4),D4,NOT(C4))))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <f>INT(OR(AND(NOT(C4),D4),AND(NOT(D4),B4)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <f>INT(AND(NOT(B4),D4))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I4" s="25"/>
@@ -4786,19 +4910,19 @@
         <v>0</v>
       </c>
       <c r="E5" s="12">
-        <f>INT(OR(AND(NOT(C5),D5),AND(C5,NOT(D5),A5)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F5" s="15">
-        <f>INT(OR(AND(A5,NOT(D5),NOT(C5)),AND(NOT(A5),D5,NOT(C5))))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G5" s="2">
-        <f>INT(OR(AND(NOT(C5),D5),AND(NOT(D5),B5)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H5" s="2">
-        <f>INT(AND(NOT(B5),D5))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I5" s="25"/>
@@ -4829,19 +4953,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="12">
-        <f>INT(OR(AND(NOT(C6),D6),AND(C6,NOT(D6),A6)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F6" s="15">
-        <f>INT(OR(AND(A6,NOT(D6),NOT(C6)),AND(NOT(A6),D6,NOT(C6))))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <f>INT(OR(AND(NOT(C6),D6),AND(NOT(D6),B6)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <f>INT(AND(NOT(B6),D6))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I6" s="25"/>
@@ -4864,19 +4988,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="12">
-        <f>INT(OR(AND(NOT(C7),D7),AND(C7,NOT(D7),A7)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F7" s="15">
-        <f>INT(OR(AND(A7,NOT(D7),NOT(C7)),AND(NOT(A7),D7,NOT(C7))))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <f>INT(OR(AND(NOT(C7),D7),AND(NOT(D7),B7)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <f>INT(AND(NOT(B7),D7))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I7" s="25"/>
@@ -4899,19 +5023,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="12">
-        <f>INT(OR(AND(NOT(C8),D8),AND(C8,NOT(D8),A8)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F8" s="15">
-        <f>INT(OR(AND(A8,NOT(D8),NOT(C8)),AND(NOT(A8),D8,NOT(C8))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G8" s="2">
-        <f>INT(OR(AND(NOT(C8),D8),AND(NOT(D8),B8)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <f>INT(AND(NOT(B8),D8))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I8" s="25"/>
@@ -4934,19 +5058,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="12">
-        <f>INT(OR(AND(NOT(C9),D9),AND(C9,NOT(D9),A9)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F9" s="15">
-        <f>INT(OR(AND(A9,NOT(D9),NOT(C9)),AND(NOT(A9),D9,NOT(C9))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <f>INT(OR(AND(NOT(C9),D9),AND(NOT(D9),B9)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <f>INT(AND(NOT(B9),D9))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I9" s="25"/>
@@ -4969,19 +5093,19 @@
         <v>0</v>
       </c>
       <c r="E10" s="12">
-        <f>INT(OR(AND(NOT(C10),D10),AND(C10,NOT(D10),A10)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" s="15">
-        <f>INT(OR(AND(A10,NOT(D10),NOT(C10)),AND(NOT(A10),D10,NOT(C10))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G10" s="2">
-        <f>INT(OR(AND(NOT(C10),D10),AND(NOT(D10),B10)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <f>INT(AND(NOT(B10),D10))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I10" s="25"/>
@@ -5004,19 +5128,19 @@
         <v>0</v>
       </c>
       <c r="E11" s="12">
-        <f>INT(OR(AND(NOT(C11),D11),AND(C11,NOT(D11),A11)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="15">
-        <f>INT(OR(AND(A11,NOT(D11),NOT(C11)),AND(NOT(A11),D11,NOT(C11))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11" s="2">
-        <f>INT(OR(AND(NOT(C11),D11),AND(NOT(D11),B11)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <f>INT(AND(NOT(B11),D11))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I11" s="25"/>
@@ -5039,19 +5163,19 @@
         <v>0</v>
       </c>
       <c r="E12" s="12">
-        <f>INT(OR(AND(NOT(C12),D12),AND(C12,NOT(D12),A12)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F12" s="15">
-        <f>INT(OR(AND(A12,NOT(D12),NOT(C12)),AND(NOT(A12),D12,NOT(C12))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G12" s="2">
-        <f>INT(OR(AND(NOT(C12),D12),AND(NOT(D12),B12)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H12" s="2">
-        <f>INT(AND(NOT(B12),D12))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I12" s="25"/>
@@ -5074,19 +5198,19 @@
         <v>0</v>
       </c>
       <c r="E13" s="12">
-        <f>INT(OR(AND(NOT(C13),D13),AND(C13,NOT(D13),A13)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F13" s="15">
-        <f>INT(OR(AND(A13,NOT(D13),NOT(C13)),AND(NOT(A13),D13,NOT(C13))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G13" s="2">
-        <f>INT(OR(AND(NOT(C13),D13),AND(NOT(D13),B13)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H13" s="2">
-        <f>INT(AND(NOT(B13),D13))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13" s="25"/>
@@ -5109,19 +5233,19 @@
         <v>1</v>
       </c>
       <c r="E14" s="12">
-        <f>INT(OR(AND(NOT(C14),D14),AND(C14,NOT(D14),A14)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" s="15">
-        <f>INT(OR(AND(A14,NOT(D14),NOT(C14)),AND(NOT(A14),D14,NOT(C14))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <f>INT(OR(AND(NOT(C14),D14),AND(NOT(D14),B14)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H14" s="2">
-        <f>INT(AND(NOT(B14),D14))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I14" s="25"/>
@@ -5144,19 +5268,19 @@
         <v>1</v>
       </c>
       <c r="E15" s="12">
-        <f>INT(OR(AND(NOT(C15),D15),AND(C15,NOT(D15),A15)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" s="15">
-        <f>INT(OR(AND(A15,NOT(D15),NOT(C15)),AND(NOT(A15),D15,NOT(C15))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <f>INT(OR(AND(NOT(C15),D15),AND(NOT(D15),B15)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H15" s="2">
-        <f>INT(AND(NOT(B15),D15))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I15" s="25"/>
@@ -5179,19 +5303,19 @@
         <v>1</v>
       </c>
       <c r="E16" s="12">
-        <f>INT(OR(AND(NOT(C16),D16),AND(C16,NOT(D16),A16)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16" s="15">
-        <f>INT(OR(AND(A16,NOT(D16),NOT(C16)),AND(NOT(A16),D16,NOT(C16))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <f>INT(OR(AND(NOT(C16),D16),AND(NOT(D16),B16)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H16" s="2">
-        <f>INT(AND(NOT(B16),D16))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I16" s="25"/>
@@ -5214,19 +5338,19 @@
         <v>1</v>
       </c>
       <c r="E17" s="19">
-        <f>INT(OR(AND(NOT(C17),D17),AND(C17,NOT(D17),A17)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17" s="10">
-        <f>INT(OR(AND(A17,NOT(D17),NOT(C17)),AND(NOT(A17),D17,NOT(C17))))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G17" s="2">
-        <f>INT(OR(AND(NOT(C17),D17),AND(NOT(D17),B17)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H17" s="2">
-        <f>INT(AND(NOT(B17),D17))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17" s="25"/>
@@ -5250,9 +5374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:O2"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5260,93 +5384,93 @@
     <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="78" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="75" t="s">
+      <c r="D1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="75" t="s">
+      <c r="I1" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="76" t="s">
+      <c r="J1" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="76" t="s">
+      <c r="L1" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="M1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="76" t="s">
+      <c r="N1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="77" t="s">
+      <c r="O1" s="70" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="32" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="33"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="73"/>
       <c r="O3" s="21" t="s">
         <v>19</v>
       </c>
@@ -5394,120 +5518,120 @@
       <c r="N4" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="50" t="s">
+      <c r="O4" s="43" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="51">
-        <v>1</v>
-      </c>
-      <c r="B5" s="52">
-        <v>1</v>
-      </c>
-      <c r="C5" s="52">
-        <v>0</v>
-      </c>
-      <c r="D5" s="52">
-        <v>0</v>
-      </c>
-      <c r="E5" s="52">
-        <v>0</v>
-      </c>
-      <c r="F5" s="52">
-        <v>0</v>
-      </c>
-      <c r="G5" s="52">
-        <v>0</v>
-      </c>
-      <c r="H5" s="53">
-        <v>0</v>
-      </c>
-      <c r="I5" s="52">
-        <f>L5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="54">
-        <f>IF(B5,0,IF(C5="↑",IF(G5,H5,INT(OR(AND(NOT(J4),K4),AND(J4,NOT(K4),D5)))),J4))</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="54">
-        <f>IF(B5,0,IF(C5="↑",IF(G5,J4,INT(OR(AND(D5,NOT(K4),NOT(J4)),AND(NOT(D5),K4,NOT(J4))))),K4))</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="52">
-        <f>IF(B5,0,IF(C5="↑",IF(G5,K4,INT(IF(J4,AND(K4,F5),L4))),L4))</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="54">
-        <f>INT(OR(AND(NOT(J5),K5),AND(NOT(K5),E5)))</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="54">
-        <f>INT(AND(NOT(E5),K5))</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="55" t="s">
+      <c r="A5" s="44">
+        <v>1</v>
+      </c>
+      <c r="B5" s="45">
+        <v>1</v>
+      </c>
+      <c r="C5" s="45">
+        <v>0</v>
+      </c>
+      <c r="D5" s="45">
+        <v>0</v>
+      </c>
+      <c r="E5" s="45">
+        <v>0</v>
+      </c>
+      <c r="F5" s="45">
+        <v>0</v>
+      </c>
+      <c r="G5" s="45">
+        <v>0</v>
+      </c>
+      <c r="H5" s="46">
+        <v>0</v>
+      </c>
+      <c r="I5" s="45">
+        <f t="shared" ref="I5:I20" si="0">L5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="47">
+        <f t="shared" ref="J5:J20" si="1">IF(B5,0,IF(C5="↑",IF(G5,H5,INT(OR(AND(NOT(J4),K4),AND(J4,NOT(K4),D5)))),J4))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="47">
+        <f t="shared" ref="K5:K20" si="2">IF(B5,0,IF(C5="↑",IF(G5,J4,INT(OR(AND(D5,NOT(K4),NOT(J4)),AND(NOT(D5),K4,NOT(J4))))),K4))</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="45">
+        <f t="shared" ref="L5:L20" si="3">IF(B5,0,IF(C5="↑",IF(G5,K4,INT(IF(J4,AND(K4,F5),L4))),L4))</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="47">
+        <f t="shared" ref="M5:M20" si="4">INT(OR(AND(NOT(J5),K5),AND(NOT(K5),E5)))</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="47">
+        <f t="shared" ref="N5:N20" si="5">INT(AND(NOT(E5),K5))</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="48" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="56">
+      <c r="A6" s="49">
         <f>A5+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="57">
-        <v>0</v>
-      </c>
-      <c r="C6" s="57">
-        <v>0</v>
-      </c>
-      <c r="D6" s="57">
-        <v>0</v>
-      </c>
-      <c r="E6" s="57">
-        <v>0</v>
-      </c>
-      <c r="F6" s="57">
-        <v>0</v>
-      </c>
-      <c r="G6" s="57">
-        <v>0</v>
-      </c>
-      <c r="H6" s="58">
-        <v>0</v>
-      </c>
-      <c r="I6" s="57">
-        <f>L6</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="59">
-        <f>IF(B6,0,IF(C6="↑",IF(G6,H6,INT(OR(AND(NOT(J5),K5),AND(J5,NOT(K5),D6)))),J5))</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="59">
-        <f>IF(B6,0,IF(C6="↑",IF(G6,J5,INT(OR(AND(D6,NOT(K5),NOT(J5)),AND(NOT(D6),K5,NOT(J5))))),K5))</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="57">
-        <f>IF(B6,0,IF(C6="↑",IF(G6,K5,INT(IF(J5,AND(K5,F6),L5))),L5))</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="59">
-        <f>INT(OR(AND(NOT(J6),K6),AND(NOT(K6),E6)))</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="59">
-        <f>INT(AND(NOT(E6),K6))</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="60" t="s">
+      <c r="B6" s="50">
+        <v>0</v>
+      </c>
+      <c r="C6" s="50">
+        <v>0</v>
+      </c>
+      <c r="D6" s="50">
+        <v>0</v>
+      </c>
+      <c r="E6" s="50">
+        <v>0</v>
+      </c>
+      <c r="F6" s="50">
+        <v>0</v>
+      </c>
+      <c r="G6" s="50">
+        <v>0</v>
+      </c>
+      <c r="H6" s="51">
+        <v>0</v>
+      </c>
+      <c r="I6" s="50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N6" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="53" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <f t="shared" ref="A7:A40" si="0">A6+1</f>
+        <f t="shared" ref="A7:A40" si="6">A6+1</f>
         <v>3</v>
       </c>
       <c r="B7" s="5">
@@ -5532,786 +5656,786 @@
         <v>0</v>
       </c>
       <c r="I7" s="5">
-        <f>L7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J7" s="15">
-        <f>IF(B7,0,IF(C7="↑",IF(G7,H7,INT(OR(AND(NOT(J6),K6),AND(J6,NOT(K6),D7)))),J6))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K7" s="15">
-        <f>IF(B7,0,IF(C7="↑",IF(G7,J6,INT(OR(AND(D7,NOT(K6),NOT(J6)),AND(NOT(D7),K6,NOT(J6))))),K6))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L7" s="5">
-        <f>IF(B7,0,IF(C7="↑",IF(G7,K6,INT(IF(J6,AND(K6,F7),L6))),L6))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M7" s="15">
-        <f>INT(OR(AND(NOT(J7),K7),AND(NOT(K7),E7)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N7" s="15">
-        <f>INT(AND(NOT(E7),K7))</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="40" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="61">
+      <c r="A8" s="54">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="55">
+        <v>0</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="55">
+        <v>0</v>
+      </c>
+      <c r="E8" s="55">
+        <v>0</v>
+      </c>
+      <c r="F8" s="55">
+        <v>0</v>
+      </c>
+      <c r="G8" s="55">
+        <v>1</v>
+      </c>
+      <c r="H8" s="57">
+        <v>0</v>
+      </c>
+      <c r="I8" s="55">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="62">
-        <v>0</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="62">
-        <v>0</v>
-      </c>
-      <c r="E8" s="62">
-        <v>0</v>
-      </c>
-      <c r="F8" s="62">
-        <v>0</v>
-      </c>
-      <c r="G8" s="62">
-        <v>1</v>
-      </c>
-      <c r="H8" s="64">
-        <v>0</v>
-      </c>
-      <c r="I8" s="62">
-        <f>L8</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="65">
-        <f>IF(B8,0,IF(C8="↑",IF(G8,H8,INT(OR(AND(NOT(J7),K7),AND(J7,NOT(K7),D8)))),J7))</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="65">
-        <f>IF(B8,0,IF(C8="↑",IF(G8,J7,INT(OR(AND(D8,NOT(K7),NOT(J7)),AND(NOT(D8),K7,NOT(J7))))),K7))</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="62">
-        <f>IF(B8,0,IF(C8="↑",IF(G8,K7,INT(IF(J7,AND(K7,F8),L7))),L7))</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="65">
-        <f>INT(OR(AND(NOT(J8),K8),AND(NOT(K8),E8)))</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="65">
-        <f>INT(AND(NOT(E8),K8))</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="58">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N8" s="58">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="59" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="56">
+      <c r="A9" s="49">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="60">
+        <v>0</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0</v>
+      </c>
+      <c r="E9" s="60">
+        <v>0</v>
+      </c>
+      <c r="F9" s="60">
+        <v>0</v>
+      </c>
+      <c r="G9" s="60">
+        <v>0</v>
+      </c>
+      <c r="H9" s="49">
+        <v>0</v>
+      </c>
+      <c r="I9" s="50">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="67">
-        <v>0</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="67">
-        <v>0</v>
-      </c>
-      <c r="E9" s="67">
-        <v>0</v>
-      </c>
-      <c r="F9" s="67">
-        <v>0</v>
-      </c>
-      <c r="G9" s="67">
-        <v>0</v>
-      </c>
-      <c r="H9" s="56">
-        <v>0</v>
-      </c>
-      <c r="I9" s="57">
-        <f>L9</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="59">
-        <f>IF(B9,0,IF(C9="↑",IF(G9,H9,INT(OR(AND(NOT(J8),K8),AND(J8,NOT(K8),D9)))),J8))</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="59">
-        <f>IF(B9,0,IF(C9="↑",IF(G9,J8,INT(OR(AND(D9,NOT(K8),NOT(J8)),AND(NOT(D9),K8,NOT(J8))))),K8))</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="57">
-        <f>IF(B9,0,IF(C9="↑",IF(G9,K8,INT(IF(J8,AND(K8,F9),L8))),L8))</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="59">
-        <f>INT(OR(AND(NOT(J9),K9),AND(NOT(K9),E9)))</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="59">
-        <f>INT(AND(NOT(E9),K9))</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="52">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="62" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <f>L10</f>
         <v>0</v>
       </c>
       <c r="J10" s="15">
-        <f>IF(B10,0,IF(C10="↑",IF(G10,H10,INT(OR(AND(NOT(J9),K9),AND(J9,NOT(K9),D10)))),J9))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" s="15">
-        <f>IF(B10,0,IF(C10="↑",IF(G10,J9,INT(OR(AND(D10,NOT(K9),NOT(J9)),AND(NOT(D10),K9,NOT(J9))))),K9))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L10" s="5">
-        <f>IF(B10,0,IF(C10="↑",IF(G10,K9,INT(IF(J9,AND(K9,F10),L9))),L9))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M10" s="15">
-        <f>INT(OR(AND(NOT(J10),K10),AND(NOT(K10),E10)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N10" s="15">
-        <f>INT(AND(NOT(E10),K10))</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="49" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="42" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="30">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B11" s="30">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>1</v>
-      </c>
-      <c r="H11" s="9">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <f>L11</f>
         <v>0</v>
       </c>
       <c r="J11" s="15">
-        <f>IF(B11,0,IF(C11="↑",IF(G11,H11,INT(OR(AND(NOT(J10),K10),AND(J10,NOT(K10),D11)))),J10))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" s="15">
-        <f>IF(B11,0,IF(C11="↑",IF(G11,J10,INT(OR(AND(D11,NOT(K10),NOT(J10)),AND(NOT(D11),K10,NOT(J10))))),K10))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L11" s="5">
-        <f>IF(B11,0,IF(C11="↑",IF(G11,K10,INT(IF(J10,AND(K10,F11),L10))),L10))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M11" s="15">
-        <f>INT(OR(AND(NOT(J11),K11),AND(NOT(K11),E11)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N11" s="15">
-        <f>INT(AND(NOT(E11),K11))</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="49" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="42" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="61">
+      <c r="A12" s="54">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="63">
+        <v>0</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="63">
+        <v>0</v>
+      </c>
+      <c r="E12" s="55">
+        <v>0</v>
+      </c>
+      <c r="F12" s="63">
+        <v>0</v>
+      </c>
+      <c r="G12" s="63">
+        <v>1</v>
+      </c>
+      <c r="H12" s="54">
+        <v>0</v>
+      </c>
+      <c r="I12" s="55">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="70">
-        <v>0</v>
-      </c>
-      <c r="C12" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="70">
-        <v>0</v>
-      </c>
-      <c r="E12" s="62">
-        <v>0</v>
-      </c>
-      <c r="F12" s="70">
-        <v>0</v>
-      </c>
-      <c r="G12" s="70">
-        <v>1</v>
-      </c>
-      <c r="H12" s="61">
-        <v>0</v>
-      </c>
-      <c r="I12" s="62">
-        <f>L12</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="65">
-        <f>IF(B12,0,IF(C12="↑",IF(G12,H12,INT(OR(AND(NOT(J11),K11),AND(J11,NOT(K11),D12)))),J11))</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="65">
-        <f>IF(B12,0,IF(C12="↑",IF(G12,J11,INT(OR(AND(D12,NOT(K11),NOT(J11)),AND(NOT(D12),K11,NOT(J11))))),K11))</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="62">
-        <f>IF(B12,0,IF(C12="↑",IF(G12,K11,INT(IF(J11,AND(K11,F12),L11))),L11))</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="65">
-        <f>INT(OR(AND(NOT(J12),K12),AND(NOT(K12),E12)))</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="65">
-        <f>INT(AND(NOT(E12),K12))</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="71"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="58">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="58">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="64"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
-        <f>L13</f>
         <v>0</v>
       </c>
       <c r="J13" s="15">
-        <f>IF(B13,0,IF(C13="↑",IF(G13,H13,INT(OR(AND(NOT(J12),K12),AND(J12,NOT(K12),D13)))),J12))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K13" s="15">
-        <f>IF(B13,0,IF(C13="↑",IF(G13,J12,INT(OR(AND(D13,NOT(K12),NOT(J12)),AND(NOT(D13),K12,NOT(J12))))),K12))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L13" s="5">
-        <f>IF(B13,0,IF(C13="↑",IF(G13,K12,INT(IF(J12,AND(K12,F13),L12))),L12))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M13" s="15">
-        <f>INT(OR(AND(NOT(J13),K13),AND(NOT(K13),E13)))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N13" s="15">
-        <f>INT(AND(NOT(E13),K13))</f>
-        <v>1</v>
-      </c>
-      <c r="O13" s="39" t="s">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O13" s="32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="8">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5">
-        <f>L14</f>
         <v>1</v>
       </c>
       <c r="J14" s="15">
-        <f>IF(B14,0,IF(C14="↑",IF(G14,H14,INT(OR(AND(NOT(J13),K13),AND(J13,NOT(K13),D14)))),J13))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K14" s="15">
-        <f>IF(B14,0,IF(C14="↑",IF(G14,J13,INT(OR(AND(D14,NOT(K13),NOT(J13)),AND(NOT(D14),K13,NOT(J13))))),K13))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L14" s="5">
-        <f>IF(B14,0,IF(C14="↑",IF(G14,K13,INT(IF(J13,AND(K13,F14),L13))),L13))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M14" s="15">
-        <f>INT(OR(AND(NOT(J14),K14),AND(NOT(K14),E14)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N14" s="15">
-        <f>INT(AND(NOT(E14),K14))</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="39" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="32" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1</v>
-      </c>
-      <c r="H15" s="6">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5">
-        <f>L15</f>
         <v>0</v>
       </c>
       <c r="J15" s="15">
-        <f>IF(B15,0,IF(C15="↑",IF(G15,H15,INT(OR(AND(NOT(J14),K14),AND(J14,NOT(K14),D15)))),J14))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K15" s="15">
-        <f>IF(B15,0,IF(C15="↑",IF(G15,J14,INT(OR(AND(D15,NOT(K14),NOT(J14)),AND(NOT(D15),K14,NOT(J14))))),K14))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L15" s="5">
-        <f>IF(B15,0,IF(C15="↑",IF(G15,K14,INT(IF(J14,AND(K14,F15),L14))),L14))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M15" s="15">
-        <f>INT(OR(AND(NOT(J15),K15),AND(NOT(K15),E15)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N15" s="15">
-        <f>INT(AND(NOT(E15),K15))</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="39" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="61">
+      <c r="A16" s="54">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="63">
+        <v>0</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="63">
+        <v>0</v>
+      </c>
+      <c r="E16" s="55">
+        <v>0</v>
+      </c>
+      <c r="F16" s="63">
+        <v>0</v>
+      </c>
+      <c r="G16" s="63">
+        <v>1</v>
+      </c>
+      <c r="H16" s="54">
+        <v>0</v>
+      </c>
+      <c r="I16" s="55">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B16" s="70">
-        <v>0</v>
-      </c>
-      <c r="C16" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="70">
-        <v>0</v>
-      </c>
-      <c r="E16" s="62">
-        <v>0</v>
-      </c>
-      <c r="F16" s="70">
-        <v>0</v>
-      </c>
-      <c r="G16" s="70">
-        <v>1</v>
-      </c>
-      <c r="H16" s="61">
-        <v>0</v>
-      </c>
-      <c r="I16" s="62">
-        <f>L16</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="65">
-        <f>IF(B16,0,IF(C16="↑",IF(G16,H16,INT(OR(AND(NOT(J15),K15),AND(J15,NOT(K15),D16)))),J15))</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="65">
-        <f>IF(B16,0,IF(C16="↑",IF(G16,J15,INT(OR(AND(D16,NOT(K15),NOT(J15)),AND(NOT(D16),K15,NOT(J15))))),K15))</f>
-        <v>1</v>
-      </c>
-      <c r="L16" s="62">
-        <f>IF(B16,0,IF(C16="↑",IF(G16,K15,INT(IF(J15,AND(K15,F16),L15))),L15))</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="65">
-        <f>INT(OR(AND(NOT(J16),K16),AND(NOT(K16),E16)))</f>
-        <v>1</v>
-      </c>
-      <c r="N16" s="65">
-        <f>INT(AND(NOT(E16),K16))</f>
-        <v>1</v>
-      </c>
-      <c r="O16" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="58">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L16" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="58">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N16" s="58">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="59"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <f>L17</f>
         <v>0</v>
       </c>
       <c r="J17" s="15">
-        <f>IF(B17,0,IF(C17="↑",IF(G17,H17,INT(OR(AND(NOT(J16),K16),AND(J16,NOT(K16),D17)))),J16))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K17" s="15">
-        <f>IF(B17,0,IF(C17="↑",IF(G17,J16,INT(OR(AND(D17,NOT(K16),NOT(J16)),AND(NOT(D17),K16,NOT(J16))))),K16))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L17" s="5">
-        <f>IF(B17,0,IF(C17="↑",IF(G17,K16,INT(IF(J16,AND(K16,F17),L16))),L16))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M17" s="15">
-        <f>INT(OR(AND(NOT(J17),K17),AND(NOT(K17),E17)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N17" s="15">
-        <f>INT(AND(NOT(E17),K17))</f>
-        <v>0</v>
-      </c>
-      <c r="O17" s="39" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="32" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B18" s="8">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>1</v>
-      </c>
-      <c r="H18" s="9">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <f>L18</f>
         <v>0</v>
       </c>
       <c r="J18" s="15">
-        <f>IF(B18,0,IF(C18="↑",IF(G18,H18,INT(OR(AND(NOT(J17),K17),AND(J17,NOT(K17),D18)))),J17))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K18" s="15">
-        <f>IF(B18,0,IF(C18="↑",IF(G18,J17,INT(OR(AND(D18,NOT(K17),NOT(J17)),AND(NOT(D18),K17,NOT(J17))))),K17))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L18" s="5">
-        <f>IF(B18,0,IF(C18="↑",IF(G18,K17,INT(IF(J17,AND(K17,F18),L17))),L17))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M18" s="15">
-        <f>INT(OR(AND(NOT(J18),K18),AND(NOT(K18),E18)))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N18" s="15">
-        <f>INT(AND(NOT(E18),K18))</f>
-        <v>1</v>
-      </c>
-      <c r="O18" s="39" t="s">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="32" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
-      </c>
-      <c r="H19" s="6">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5">
-        <f>L19</f>
         <v>1</v>
       </c>
       <c r="J19" s="15">
-        <f>IF(B19,0,IF(C19="↑",IF(G19,H19,INT(OR(AND(NOT(J18),K18),AND(J18,NOT(K18),D19)))),J18))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K19" s="15">
-        <f>IF(B19,0,IF(C19="↑",IF(G19,J18,INT(OR(AND(D19,NOT(K18),NOT(J18)),AND(NOT(D19),K18,NOT(J18))))),K18))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L19" s="5">
-        <f>IF(B19,0,IF(C19="↑",IF(G19,K18,INT(IF(J18,AND(K18,F19),L18))),L18))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M19" s="15">
-        <f>INT(OR(AND(NOT(J19),K19),AND(NOT(K19),E19)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N19" s="15">
-        <f>INT(AND(NOT(E19),K19))</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="39" t="s">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="32" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="64">
+      <c r="A20" s="57">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="63">
+        <v>0</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="63">
+        <v>0</v>
+      </c>
+      <c r="E20" s="55">
+        <v>0</v>
+      </c>
+      <c r="F20" s="55">
+        <v>0</v>
+      </c>
+      <c r="G20" s="55">
+        <v>1</v>
+      </c>
+      <c r="H20" s="57">
+        <v>0</v>
+      </c>
+      <c r="I20" s="55">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B20" s="70">
-        <v>0</v>
-      </c>
-      <c r="C20" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="70">
-        <v>0</v>
-      </c>
-      <c r="E20" s="62">
-        <v>0</v>
-      </c>
-      <c r="F20" s="62">
-        <v>0</v>
-      </c>
-      <c r="G20" s="62">
-        <v>1</v>
-      </c>
-      <c r="H20" s="64">
-        <v>0</v>
-      </c>
-      <c r="I20" s="62">
-        <f>L20</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="65">
-        <f>IF(B20,0,IF(C20="↑",IF(G20,H20,INT(OR(AND(NOT(J19),K19),AND(J19,NOT(K19),D20)))),J19))</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="65">
-        <f>IF(B20,0,IF(C20="↑",IF(G20,J19,INT(OR(AND(D20,NOT(K19),NOT(J19)),AND(NOT(D20),K19,NOT(J19))))),K19))</f>
-        <v>1</v>
-      </c>
-      <c r="L20" s="62">
-        <f>IF(B20,0,IF(C20="↑",IF(G20,K19,INT(IF(J19,AND(K19,F20),L19))),L19))</f>
-        <v>0</v>
-      </c>
-      <c r="M20" s="65">
-        <f>INT(OR(AND(NOT(J20),K20),AND(NOT(K20),E20)))</f>
-        <v>1</v>
-      </c>
-      <c r="N20" s="65">
-        <f>INT(AND(NOT(E20),K20))</f>
-        <v>1</v>
-      </c>
-      <c r="O20" s="66"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="58">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="58">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N20" s="58">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="59"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="56">
-        <f t="shared" si="0"/>
+      <c r="A21" s="49">
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="B21" s="67">
-        <v>0</v>
-      </c>
-      <c r="C21" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="67">
-        <v>0</v>
-      </c>
-      <c r="E21" s="67">
-        <v>0</v>
-      </c>
-      <c r="F21" s="67">
-        <v>0</v>
-      </c>
-      <c r="G21" s="67">
-        <v>0</v>
-      </c>
-      <c r="H21" s="56">
-        <v>0</v>
-      </c>
-      <c r="I21" s="57">
-        <f t="shared" ref="I21:I28" si="1">L21</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="59">
-        <f t="shared" ref="J21:J28" si="2">IF(B21,0,IF(C21="↑",IF(G21,H21,INT(OR(AND(NOT(J20),K20),AND(J20,NOT(K20),D21)))),J20))</f>
-        <v>1</v>
-      </c>
-      <c r="K21" s="59">
-        <f t="shared" ref="K21:K28" si="3">IF(B21,0,IF(C21="↑",IF(G21,J20,INT(OR(AND(D21,NOT(K20),NOT(J20)),AND(NOT(D21),K20,NOT(J20))))),K20))</f>
-        <v>1</v>
-      </c>
-      <c r="L21" s="57">
-        <f t="shared" ref="L21:L28" si="4">IF(B21,0,IF(C21="↑",IF(G21,K20,INT(IF(J20,AND(K20,F21),L20))),L20))</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="59">
-        <f t="shared" ref="M21:M28" si="5">INT(OR(AND(NOT(J21),K21),AND(NOT(K21),E21)))</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="59">
-        <f t="shared" ref="N21:N28" si="6">INT(AND(NOT(E21),K21))</f>
-        <v>1</v>
-      </c>
-      <c r="O21" s="72" t="s">
+      <c r="B21" s="60">
+        <v>0</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="60">
+        <v>0</v>
+      </c>
+      <c r="E21" s="60">
+        <v>0</v>
+      </c>
+      <c r="F21" s="60">
+        <v>0</v>
+      </c>
+      <c r="G21" s="60">
+        <v>0</v>
+      </c>
+      <c r="H21" s="49">
+        <v>0</v>
+      </c>
+      <c r="I21" s="50">
+        <f t="shared" ref="I21:I28" si="7">L21</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="52">
+        <f t="shared" ref="J21:J28" si="8">IF(B21,0,IF(C21="↑",IF(G21,H21,INT(OR(AND(NOT(J20),K20),AND(J20,NOT(K20),D21)))),J20))</f>
+        <v>1</v>
+      </c>
+      <c r="K21" s="52">
+        <f t="shared" ref="K21:K28" si="9">IF(B21,0,IF(C21="↑",IF(G21,J20,INT(OR(AND(D21,NOT(K20),NOT(J20)),AND(NOT(D21),K20,NOT(J20))))),K20))</f>
+        <v>1</v>
+      </c>
+      <c r="L21" s="50">
+        <f t="shared" ref="L21:L28" si="10">IF(B21,0,IF(C21="↑",IF(G21,K20,INT(IF(J20,AND(K20,F21),L20))),L20))</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="52">
+        <f t="shared" ref="M21:M28" si="11">INT(OR(AND(NOT(J21),K21),AND(NOT(K21),E21)))</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="52">
+        <f t="shared" ref="N21:N28" si="12">INT(AND(NOT(E21),K21))</f>
+        <v>1</v>
+      </c>
+      <c r="O21" s="65" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="B22" s="8">
@@ -6336,36 +6460,36 @@
         <v>0</v>
       </c>
       <c r="I22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J22" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K22" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="L22" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="M22" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="N22" s="15">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="O22" s="40" t="s">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="O22" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="B23" s="8">
@@ -6390,94 +6514,94 @@
         <v>0</v>
       </c>
       <c r="I23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J23" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K23" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L23" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="M23" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N23" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="54">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="61">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B24" s="70">
-        <v>0</v>
-      </c>
-      <c r="C24" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="70">
-        <v>0</v>
-      </c>
-      <c r="E24" s="70">
-        <v>0</v>
-      </c>
-      <c r="F24" s="70">
-        <v>0</v>
-      </c>
-      <c r="G24" s="70">
-        <v>1</v>
-      </c>
-      <c r="H24" s="61">
-        <v>1</v>
-      </c>
-      <c r="I24" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="65">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K24" s="65">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="62">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="65">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="65">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="73"/>
+      <c r="B24" s="63">
+        <v>0</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="63">
+        <v>0</v>
+      </c>
+      <c r="E24" s="63">
+        <v>0</v>
+      </c>
+      <c r="F24" s="63">
+        <v>0</v>
+      </c>
+      <c r="G24" s="63">
+        <v>1</v>
+      </c>
+      <c r="H24" s="54">
+        <v>1</v>
+      </c>
+      <c r="I24" s="55">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="58">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="55">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="58">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="58">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="66"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="B25" s="8">
         <v>0</v>
       </c>
-      <c r="C25" s="68" t="s">
+      <c r="C25" s="61" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="8">
@@ -6496,36 +6620,36 @@
         <v>0</v>
       </c>
       <c r="I25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J25" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K25" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M25" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N25" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="40" t="s">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="B26" s="8">
@@ -6550,36 +6674,36 @@
         <v>0</v>
       </c>
       <c r="I26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J26" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K26" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M26" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N26" s="15">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="40" t="s">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="33" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="B27" s="8">
@@ -6604,142 +6728,142 @@
         <v>0</v>
       </c>
       <c r="I27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K27" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M27" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N27" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="54">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="61">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B28" s="70">
-        <v>0</v>
-      </c>
-      <c r="C28" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="70">
-        <v>0</v>
-      </c>
-      <c r="E28" s="70">
-        <v>0</v>
-      </c>
-      <c r="F28" s="70">
-        <v>0</v>
-      </c>
-      <c r="G28" s="70">
-        <v>1</v>
-      </c>
-      <c r="H28" s="61">
-        <v>1</v>
-      </c>
-      <c r="I28" s="62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="65">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="K28" s="65">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L28" s="62">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M28" s="65">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="65">
+      <c r="B28" s="63">
+        <v>0</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="63">
+        <v>0</v>
+      </c>
+      <c r="E28" s="63">
+        <v>0</v>
+      </c>
+      <c r="F28" s="63">
+        <v>0</v>
+      </c>
+      <c r="G28" s="63">
+        <v>1</v>
+      </c>
+      <c r="H28" s="54">
+        <v>1</v>
+      </c>
+      <c r="I28" s="55">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="58">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="58">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="55">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="58">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="58">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="66"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="49">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="73"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="56">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B29" s="67">
-        <v>0</v>
-      </c>
-      <c r="C29" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="67">
-        <v>1</v>
-      </c>
-      <c r="E29" s="67">
-        <v>0</v>
-      </c>
-      <c r="F29" s="67">
-        <v>0</v>
-      </c>
-      <c r="G29" s="67">
-        <v>0</v>
-      </c>
-      <c r="H29" s="56">
-        <v>0</v>
-      </c>
-      <c r="I29" s="57">
-        <f t="shared" ref="I29:I32" si="7">L29</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="59">
-        <f t="shared" ref="J29:J32" si="8">IF(B29,0,IF(C29="↑",IF(G29,H29,INT(OR(AND(NOT(J28),K28),AND(J28,NOT(K28),D29)))),J28))</f>
-        <v>1</v>
-      </c>
-      <c r="K29" s="59">
-        <f t="shared" ref="K29:K32" si="9">IF(B29,0,IF(C29="↑",IF(G29,J28,INT(OR(AND(D29,NOT(K28),NOT(J28)),AND(NOT(D29),K28,NOT(J28))))),K28))</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="57">
-        <f t="shared" ref="L29:L32" si="10">IF(B29,0,IF(C29="↑",IF(G29,K28,INT(IF(J28,AND(K28,F29),L28))),L28))</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="59">
-        <f t="shared" ref="M29:M32" si="11">INT(OR(AND(NOT(J29),K29),AND(NOT(K29),E29)))</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="59">
-        <f t="shared" ref="N29:N32" si="12">INT(AND(NOT(E29),K29))</f>
-        <v>0</v>
-      </c>
-      <c r="O29" s="72" t="s">
+      <c r="B29" s="60">
+        <v>0</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="60">
+        <v>1</v>
+      </c>
+      <c r="E29" s="60">
+        <v>0</v>
+      </c>
+      <c r="F29" s="60">
+        <v>0</v>
+      </c>
+      <c r="G29" s="60">
+        <v>0</v>
+      </c>
+      <c r="H29" s="49">
+        <v>0</v>
+      </c>
+      <c r="I29" s="50">
+        <f t="shared" ref="I29:I32" si="13">L29</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="52">
+        <f t="shared" ref="J29:J32" si="14">IF(B29,0,IF(C29="↑",IF(G29,H29,INT(OR(AND(NOT(J28),K28),AND(J28,NOT(K28),D29)))),J28))</f>
+        <v>1</v>
+      </c>
+      <c r="K29" s="52">
+        <f t="shared" ref="K29:K32" si="15">IF(B29,0,IF(C29="↑",IF(G29,J28,INT(OR(AND(D29,NOT(K28),NOT(J28)),AND(NOT(D29),K28,NOT(J28))))),K28))</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="50">
+        <f t="shared" ref="L29:L32" si="16">IF(B29,0,IF(C29="↑",IF(G29,K28,INT(IF(J28,AND(K28,F29),L28))),L28))</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="52">
+        <f t="shared" ref="M29:M32" si="17">INT(OR(AND(NOT(J29),K29),AND(NOT(K29),E29)))</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="52">
+        <f t="shared" ref="N29:N32" si="18">INT(AND(NOT(E29),K29))</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="65" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="B30" s="8">
@@ -6764,36 +6888,36 @@
         <v>0</v>
       </c>
       <c r="I30" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J30" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K30" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M30" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="N30" s="15">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="O30" s="40" t="s">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="O30" s="33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="B31" s="8">
@@ -6818,142 +6942,142 @@
         <v>1</v>
       </c>
       <c r="I31" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="J31" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="K31" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="M31" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N31" s="15">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="40" t="s">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="33" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="61">
-        <f t="shared" si="0"/>
+      <c r="A32" s="54">
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="B32" s="70">
-        <v>0</v>
-      </c>
-      <c r="C32" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="70">
-        <v>0</v>
-      </c>
-      <c r="E32" s="70">
-        <v>0</v>
-      </c>
-      <c r="F32" s="70">
-        <v>0</v>
-      </c>
-      <c r="G32" s="70">
-        <v>1</v>
-      </c>
-      <c r="H32" s="61">
-        <v>1</v>
-      </c>
-      <c r="I32" s="62">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="65">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="K32" s="65">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="L32" s="62">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="65">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="65">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="O32" s="73"/>
+      <c r="B32" s="63">
+        <v>0</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="63">
+        <v>0</v>
+      </c>
+      <c r="E32" s="63">
+        <v>0</v>
+      </c>
+      <c r="F32" s="63">
+        <v>0</v>
+      </c>
+      <c r="G32" s="63">
+        <v>1</v>
+      </c>
+      <c r="H32" s="54">
+        <v>1</v>
+      </c>
+      <c r="I32" s="55">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="58">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="58">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="L32" s="55">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="58">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="58">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="O32" s="66"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="56">
-        <f t="shared" si="0"/>
+      <c r="A33" s="49">
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="B33" s="67">
-        <v>0</v>
-      </c>
-      <c r="C33" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="67">
-        <v>0</v>
-      </c>
-      <c r="E33" s="67">
-        <v>0</v>
-      </c>
-      <c r="F33" s="67">
-        <v>0</v>
-      </c>
-      <c r="G33" s="67">
-        <v>0</v>
-      </c>
-      <c r="H33" s="56">
-        <v>0</v>
-      </c>
-      <c r="I33" s="57">
-        <f t="shared" ref="I33:I40" si="13">L33</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="59">
-        <f t="shared" ref="J33:J40" si="14">IF(B33,0,IF(C33="↑",IF(G33,H33,INT(OR(AND(NOT(J32),K32),AND(J32,NOT(K32),D33)))),J32))</f>
-        <v>0</v>
-      </c>
-      <c r="K33" s="59">
-        <f t="shared" ref="K33:K40" si="15">IF(B33,0,IF(C33="↑",IF(G33,J32,INT(OR(AND(D33,NOT(K32),NOT(J32)),AND(NOT(D33),K32,NOT(J32))))),K32))</f>
-        <v>0</v>
-      </c>
-      <c r="L33" s="57">
-        <f t="shared" ref="L33:L40" si="16">IF(B33,0,IF(C33="↑",IF(G33,K32,INT(IF(J32,AND(K32,F33),L32))),L32))</f>
-        <v>0</v>
-      </c>
-      <c r="M33" s="59">
-        <f t="shared" ref="M33:M40" si="17">INT(OR(AND(NOT(J33),K33),AND(NOT(K33),E33)))</f>
-        <v>0</v>
-      </c>
-      <c r="N33" s="59">
-        <f t="shared" ref="N33:N40" si="18">INT(AND(NOT(E33),K33))</f>
-        <v>0</v>
-      </c>
-      <c r="O33" s="72" t="s">
+      <c r="B33" s="60">
+        <v>0</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="60">
+        <v>0</v>
+      </c>
+      <c r="E33" s="60">
+        <v>0</v>
+      </c>
+      <c r="F33" s="60">
+        <v>0</v>
+      </c>
+      <c r="G33" s="60">
+        <v>0</v>
+      </c>
+      <c r="H33" s="49">
+        <v>0</v>
+      </c>
+      <c r="I33" s="50">
+        <f t="shared" ref="I33:I40" si="19">L33</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="52">
+        <f t="shared" ref="J33:J40" si="20">IF(B33,0,IF(C33="↑",IF(G33,H33,INT(OR(AND(NOT(J32),K32),AND(J32,NOT(K32),D33)))),J32))</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="52">
+        <f t="shared" ref="K33:K40" si="21">IF(B33,0,IF(C33="↑",IF(G33,J32,INT(OR(AND(D33,NOT(K32),NOT(J32)),AND(NOT(D33),K32,NOT(J32))))),K32))</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="50">
+        <f t="shared" ref="L33:L40" si="22">IF(B33,0,IF(C33="↑",IF(G33,K32,INT(IF(J32,AND(K32,F33),L32))),L32))</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="52">
+        <f t="shared" ref="M33:M40" si="23">INT(OR(AND(NOT(J33),K33),AND(NOT(K33),E33)))</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="52">
+        <f t="shared" ref="N33:N40" si="24">INT(AND(NOT(E33),K33))</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="65" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
       <c r="B34" s="8">
@@ -6978,36 +7102,36 @@
         <v>0</v>
       </c>
       <c r="I34" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J34" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K34" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M34" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N34" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="O34" s="40" t="s">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="33" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="B35" s="8">
@@ -7032,142 +7156,142 @@
         <v>1</v>
       </c>
       <c r="I35" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J35" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="K35" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L35" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M35" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N35" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="40" t="s">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="33" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="61">
-        <f t="shared" si="0"/>
+      <c r="A36" s="54">
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="B36" s="70">
-        <v>0</v>
-      </c>
-      <c r="C36" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="70">
-        <v>0</v>
-      </c>
-      <c r="E36" s="70">
-        <v>0</v>
-      </c>
-      <c r="F36" s="70">
-        <v>0</v>
-      </c>
-      <c r="G36" s="70">
-        <v>1</v>
-      </c>
-      <c r="H36" s="61">
-        <v>1</v>
-      </c>
-      <c r="I36" s="62">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="65">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="K36" s="65">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="L36" s="62">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="65">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="65">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="O36" s="73"/>
+      <c r="B36" s="63">
+        <v>0</v>
+      </c>
+      <c r="C36" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="63">
+        <v>0</v>
+      </c>
+      <c r="E36" s="63">
+        <v>0</v>
+      </c>
+      <c r="F36" s="63">
+        <v>0</v>
+      </c>
+      <c r="G36" s="63">
+        <v>1</v>
+      </c>
+      <c r="H36" s="54">
+        <v>1</v>
+      </c>
+      <c r="I36" s="55">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="58">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="58">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="L36" s="55">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="58">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="58">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="O36" s="66"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
-      <c r="B37" s="67">
-        <v>0</v>
-      </c>
-      <c r="C37" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="67">
-        <v>1</v>
-      </c>
-      <c r="E37" s="67">
-        <v>0</v>
-      </c>
-      <c r="F37" s="67">
-        <v>0</v>
-      </c>
-      <c r="G37" s="67">
-        <v>0</v>
-      </c>
-      <c r="H37" s="56">
-        <v>0</v>
-      </c>
-      <c r="I37" s="57">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="59">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="K37" s="59">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="57">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="59">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="N37" s="59">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="O37" s="72" t="s">
+      <c r="B37" s="60">
+        <v>0</v>
+      </c>
+      <c r="C37" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="60">
+        <v>1</v>
+      </c>
+      <c r="E37" s="60">
+        <v>0</v>
+      </c>
+      <c r="F37" s="60">
+        <v>0</v>
+      </c>
+      <c r="G37" s="60">
+        <v>0</v>
+      </c>
+      <c r="H37" s="49">
+        <v>0</v>
+      </c>
+      <c r="I37" s="50">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="52">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="52">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="50">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="52">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="52">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="65" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="B38" s="8">
@@ -7192,36 +7316,36 @@
         <v>0</v>
       </c>
       <c r="I38" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J38" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K38" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M38" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N38" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="O38" s="40" t="s">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="33" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
       <c r="B39" s="8">
@@ -7246,36 +7370,36 @@
         <v>0</v>
       </c>
       <c r="I39" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J39" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K39" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L39" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M39" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N39" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="O39" s="40" t="s">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="33" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
       <c r="B40" s="8">
@@ -7300,30 +7424,30 @@
         <v>0</v>
       </c>
       <c r="I40" s="5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J40" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K40" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L40" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M40" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="N40" s="15">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="O40" s="40"/>
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>